<commit_message>
excel upload testing done
</commit_message>
<xml_diff>
--- a/public/uploads/suppliers-list.xlsx
+++ b/public/uploads/suppliers-list.xlsx
@@ -33,9 +33,6 @@
     <t>supplier1</t>
   </si>
   <si>
-    <t>s@s.com</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>supplier</t>
+  </si>
+  <si>
+    <t>s1@s.com</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -433,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -441,50 +441,50 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>1800000000</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1900000000</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1700000000</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>